<commit_message>
minor changes to schematic and BOM
</commit_message>
<xml_diff>
--- a/BOM-Datasheets/Micro-HAB BOM.xlsx
+++ b/BOM-Datasheets/Micro-HAB BOM.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danda\Desktop\Projects\SPEX\micro-hab\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\GitHub\micro-hab\BOM-Datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10720" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10725" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="Micro-HAB BOM Rev. 1" sheetId="2" r:id="rId1"/>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Manf Part Number</t>
   </si>
   <si>
-    <t>Manf</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
     <t>Datasheet</t>
   </si>
   <si>
-    <t>Purchase Link</t>
-  </si>
-  <si>
     <t>Footprint</t>
   </si>
   <si>
@@ -63,6 +57,18 @@
   </si>
   <si>
     <t>Micro-HAB Bill of Materials [Rev. 1]</t>
+  </si>
+  <si>
+    <t>Manfacturer</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
   </si>
 </sst>
 </file>
@@ -120,12 +126,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -333,33 +345,6 @@
     <xf numFmtId="4" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -376,6 +361,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -666,134 +678,138 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="34.54296875" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.90625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="15.36328125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.81640625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="17.6328125" style="18" customWidth="1"/>
-    <col min="7" max="7" width="40.36328125" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.90625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.54296875" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.26953125" style="18" customWidth="1"/>
-    <col min="11" max="11" width="7.453125" style="20" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" style="20" customWidth="1"/>
-    <col min="13" max="13" width="9.1796875" style="9"/>
-    <col min="14" max="15" width="9.1796875" style="1"/>
-    <col min="16" max="16" width="13.26953125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="5.85546875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="22" style="18" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="20" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="20" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="9"/>
+    <col min="14" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="13.28515625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="31"/>
+    <row r="1" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="37"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="34"/>
+    <row r="2" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="40"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="34"/>
+    <row r="3" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="40"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="37"/>
+    <row r="4" spans="1:13" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="43"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="K5" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="21" t="s">
+      <c r="L5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="22" t="s">
-        <v>10</v>
-      </c>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" s="12" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
+    <row r="6" spans="1:13" s="12" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="D6" s="19"/>
       <c r="E6" s="5"/>
@@ -801,11 +817,19 @@
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="22"/>
-    </row>
-    <row r="7" spans="1:13" s="12" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J6" s="18">
+        <v>1</v>
+      </c>
+      <c r="K6" s="20">
+        <f>IF(J6&lt;=24,4.09,IF(J6&lt;=99,3.75,IF(J6&lt;=999,3.4)))</f>
+        <v>4.09</v>
+      </c>
+      <c r="L6" s="22">
+        <f>(K6*J6)</f>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="12" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="5"/>
@@ -815,11 +839,19 @@
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="17"/>
-    </row>
-    <row r="8" spans="1:13" s="12" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J7" s="15">
+        <v>1</v>
+      </c>
+      <c r="K7" s="20">
+        <f t="shared" ref="K7:K24" si="0">IF(J7&lt;=24,4.09,IF(J7&lt;=99,3.75,IF(J7&lt;=999,3.4)))</f>
+        <v>4.09</v>
+      </c>
+      <c r="L7" s="22">
+        <f t="shared" ref="L7:L24" si="1">(K7*J7)</f>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="12" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="5"/>
@@ -829,11 +861,19 @@
       <c r="G8" s="19"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="22"/>
-    </row>
-    <row r="9" spans="1:13" s="12" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J8" s="18">
+        <v>1</v>
+      </c>
+      <c r="K8" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L8" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="12" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="5"/>
@@ -843,11 +883,19 @@
       <c r="G9" s="19"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="19"/>
-    </row>
-    <row r="10" spans="1:13" s="12" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J9" s="15">
+        <v>1</v>
+      </c>
+      <c r="K9" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L9" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="12" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="5"/>
@@ -857,11 +905,19 @@
       <c r="G10" s="19"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="22"/>
-    </row>
-    <row r="11" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J10" s="18">
+        <v>1</v>
+      </c>
+      <c r="K10" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L10" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="5"/>
@@ -871,12 +927,20 @@
       <c r="G11" s="19"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="19"/>
+      <c r="J11" s="15">
+        <v>1</v>
+      </c>
+      <c r="K11" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L11" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="5"/>
@@ -886,12 +950,20 @@
       <c r="G12" s="19"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="17"/>
+      <c r="J12" s="15">
+        <v>1</v>
+      </c>
+      <c r="K12" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L12" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="6"/>
@@ -901,12 +973,20 @@
       <c r="G13" s="19"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="17"/>
+      <c r="J13" s="15">
+        <v>1</v>
+      </c>
+      <c r="K13" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L13" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
       <c r="B14" s="14"/>
       <c r="C14" s="6"/>
@@ -916,11 +996,19 @@
       <c r="G14" s="19"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="19"/>
-    </row>
-    <row r="15" spans="1:13" s="13" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J14" s="15">
+        <v>1</v>
+      </c>
+      <c r="K14" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L14" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="13" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="B15" s="14"/>
       <c r="C15" s="6"/>
@@ -930,11 +1018,19 @@
       <c r="G15" s="19"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="19"/>
-    </row>
-    <row r="16" spans="1:13" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J15" s="15">
+        <v>1</v>
+      </c>
+      <c r="K15" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L15" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="2" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
       <c r="C16" s="5"/>
@@ -944,11 +1040,19 @@
       <c r="G16" s="19"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="22"/>
-    </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J16" s="18">
+        <v>1</v>
+      </c>
+      <c r="K16" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L16" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="6"/>
@@ -958,11 +1062,19 @@
       <c r="G17" s="19"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="22"/>
-    </row>
-    <row r="18" spans="1:13" s="12" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J17" s="18">
+        <v>1</v>
+      </c>
+      <c r="K17" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L17" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="12" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="14"/>
       <c r="C18" s="6"/>
@@ -972,11 +1084,19 @@
       <c r="G18" s="19"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="22"/>
-    </row>
-    <row r="19" spans="1:13" s="12" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J18" s="18">
+        <v>1</v>
+      </c>
+      <c r="K18" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L18" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="12" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="6"/>
@@ -986,11 +1106,19 @@
       <c r="G19" s="19"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="22"/>
-    </row>
-    <row r="20" spans="1:13" s="12" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J19" s="18">
+        <v>1</v>
+      </c>
+      <c r="K19" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L19" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="12" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="14"/>
       <c r="C20" s="6"/>
@@ -1000,11 +1128,19 @@
       <c r="G20" s="19"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="19"/>
-    </row>
-    <row r="21" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J20" s="15">
+        <v>1</v>
+      </c>
+      <c r="K20" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L20" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="14"/>
       <c r="C21" s="6"/>
@@ -1014,12 +1150,20 @@
       <c r="G21" s="19"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="19"/>
+      <c r="J21" s="15">
+        <v>1</v>
+      </c>
+      <c r="K21" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L21" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="6"/>
@@ -1029,12 +1173,20 @@
       <c r="G22" s="19"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="19"/>
+      <c r="J22" s="15">
+        <v>1</v>
+      </c>
+      <c r="K22" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L22" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" s="12" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" s="12" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="6"/>
@@ -1044,35 +1196,51 @@
       <c r="G23" s="19"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="19"/>
-    </row>
-    <row r="24" spans="1:13" s="3" customFormat="1" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J23" s="15">
+        <v>1</v>
+      </c>
+      <c r="K23" s="20">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L23" s="22">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="3" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
-      <c r="C24" s="39"/>
+      <c r="C24" s="30"/>
       <c r="D24" s="11"/>
-      <c r="E24" s="39"/>
+      <c r="E24" s="30"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="43"/>
-    </row>
-    <row r="25" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="32">
+        <v>1</v>
+      </c>
+      <c r="K24" s="33">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="L24" s="34">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
-      <c r="L25" s="38"/>
-    </row>
-    <row r="26" spans="1:13" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L25" s="29"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J26" s="23"/>
       <c r="K26" s="24"/>
       <c r="L26" s="27"/>
     </row>
-    <row r="27" spans="1:13" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:13" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J27" s="25"/>
       <c r="K27" s="26"/>
       <c r="L27" s="28"/>

</xml_diff>